<commit_message>
changes in the localgini code
</commit_message>
<xml_diff>
--- a/Thresholding/Local_gini/HK_G_acc_LG.xlsx
+++ b/Thresholding/Local_gini/HK_G_acc_LG.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>HK_G_acc_LG</t>
+  </si>
   <si>
     <t>HK_G_acc_LG</t>
   </si>
@@ -99,7 +102,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
localGini changed, closer to the final results
</commit_message>
<xml_diff>
--- a/Thresholding/Local_gini/HK_G_acc_LG.xlsx
+++ b/Thresholding/Local_gini/HK_G_acc_LG.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>HK_G_acc_LG</t>
+  </si>
   <si>
     <t>HK_G_acc_LG</t>
   </si>
@@ -117,7 +120,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Results from all the context-specific models
</commit_message>
<xml_diff>
--- a/Thresholding/Local_gini/HK_G_acc_LG.xlsx
+++ b/Thresholding/Local_gini/HK_G_acc_LG.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="34" uniqueCount="31">
   <si>
     <t>HK_G_acc_LG</t>
   </si>
@@ -167,242 +167,242 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>95.439189189189193</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>96.11486486486487</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>95.777027027027032</v>
+        <v>76.230661040787624</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>95.270270270270274</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>95.608108108108098</v>
+        <v>76.371308016877634</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>95.945945945945937</v>
+        <v>76.371308016877634</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>94.763513513513516</v>
+        <v>76.371308016877634</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>95.608108108108098</v>
+        <v>76.090014064697613</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>95.608108108108098</v>
+        <v>76.371308016877634</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>95.101351351351354</v>
+        <v>76.371308016877634</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>88.344594594594597</v>
+        <v>75.949367088607602</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>94.594594594594597</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>94.087837837837839</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>93.074324324324323</v>
+        <v>76.230661040787624</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>93.074324324324323</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>91.722972972972968</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>94.425675675675677</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>94.425675675675677</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>93.243243243243242</v>
+        <v>76.230661040787624</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>95.101351351351354</v>
+        <v>76.230661040787624</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>94.087837837837839</v>
+        <v>76.230661040787624</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>91.21621621621621</v>
+        <v>76.090014064697613</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>92.567567567567565</v>
+        <v>76.230661040787624</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>92.567567567567565</v>
+        <v>75.808720112517577</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>96.28378378378379</v>
+        <v>77.355836849507725</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>94.932432432432435</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>96.11486486486487</v>
+        <v>77.355836849507725</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>93.581081081081081</v>
+        <v>76.090014064697613</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>94.087837837837839</v>
+        <v>76.230661040787624</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>95.439189189189193</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>95.945945945945937</v>
+        <v>76.371308016877634</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>95.608108108108098</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>95.608108108108098</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>94.087837837837839</v>
+        <v>76.65260196905767</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>94.594594594594597</v>
+        <v>75.668073136427566</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>71.452702702702695</v>
+        <v>75.386779184247544</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>94.256756756756758</v>
+        <v>76.090014064697613</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>94.932432432432435</v>
+        <v>77.074542897327703</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>93.243243243243242</v>
+        <v>77.215189873417728</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>95.777027027027032</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>95.270270270270274</v>
+        <v>76.371308016877634</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>95.777027027027032</v>
+        <v>76.371308016877634</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>95.270270270270274</v>
+        <v>76.371308016877634</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>94.932432432432435</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>95.270270270270274</v>
+        <v>76.371308016877634</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>95.270270270270274</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>89.189189189189193</v>
+        <v>76.371308016877634</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>95.777027027027032</v>
+        <v>76.511954992967645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>